<commit_message>
Kr stripped vs unstripped comparison
</commit_message>
<xml_diff>
--- a/calculations/scenarious_v1_with_ecooling/combined_charge_and_isotope_scan_results/output/Combined_results_conservative_and_optimistic.xlsx
+++ b/calculations/scenarious_v1_with_ecooling/combined_charge_and_isotope_scan_results/output/Combined_results_conservative_and_optimistic.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\elias\PhD_projects\injector_model\calculations\scenarious_v1_with_ecooling\combined_charge_and_isotope_scan_results\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DCAAE5-992F-4D71-9EC6-694319A4EC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1E0A39-ECD5-4652-8A01-2B25AD77858C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2_no_PS_bunch_splitting_conserv" sheetId="4" r:id="rId1"/>
+    <sheet name="1_baseline_conservative" sheetId="4" r:id="rId1"/>
     <sheet name="2_no_PS_bunch_splitting_optimis" sheetId="2" r:id="rId2"/>
     <sheet name="Conservative_vs_optimistic" sheetId="5" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'2_no_PS_bunch_splitting_conserv'!$A$1:$J$56</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'1_baseline_conservative'!$A$1:$J$56</definedName>
     <definedName name="ExternalData_1" localSheetId="1" hidden="1">'2_no_PS_bunch_splitting_optimis'!$A$1:$J$56</definedName>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">'Conservative_vs_optimistic'!$A$1:$D$11</definedName>
   </definedNames>
@@ -2783,7 +2783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -4598,7 +4598,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>